<commit_message>
Maze Generator initial setup
</commit_message>
<xml_diff>
--- a/DTT-Test-Hour-Log.xlsx
+++ b/DTT-Test-Hour-Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Saxion Work\Internship\DTT\DTT Test - Unity - 2021\Maze-Generation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DC3853-FED5-4DF3-A94F-F8665AECD37E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35591CAB-F5B3-493F-BC2B-4BE1167C14F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Subject</t>
   </si>
@@ -48,25 +48,10 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Example 2</t>
-  </si>
-  <si>
-    <t>Had some issues with…</t>
-  </si>
-  <si>
     <t>Total amount of hours</t>
   </si>
   <si>
     <t>Bonus</t>
-  </si>
-  <si>
-    <t>Example 3</t>
-  </si>
-  <si>
-    <t>Implemented bonus feature….</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <r>
@@ -95,6 +80,18 @@
   </si>
   <si>
     <t>Reading through the DTT Test, setting up a unity scene, settuping up github repo, and reading up on Maze generation.</t>
+  </si>
+  <si>
+    <t>Setting up structure for maze generation</t>
+  </si>
+  <si>
+    <t>Creating UML diagram to plan out the handling of a perfect maze generator</t>
+  </si>
+  <si>
+    <t>Starting Creation of Maze algorithm</t>
+  </si>
+  <si>
+    <t>Original maze structure creation as setup for Prim's algorithm</t>
   </si>
 </sst>
 </file>
@@ -1712,20 +1709,20 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.46484375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.69921875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.69921875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.59765625" style="1" customWidth="1"/>
     <col min="4" max="4" width="38.59765625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="6.5" style="1" customWidth="1"/>
-    <col min="7" max="251" width="6.5" customWidth="1"/>
+    <col min="5" max="6" width="6.46484375" style="1" customWidth="1"/>
+    <col min="7" max="251" width="6.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="22"/>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -1733,9 +1730,9 @@
       <c r="E1" s="10"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -1743,7 +1740,7 @@
       <c r="E2" s="24"/>
       <c r="F2" s="25"/>
     </row>
-    <row r="3" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
@@ -1757,13 +1754,13 @@
         <v>3</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B4" s="17">
         <v>1</v>
@@ -1772,46 +1769,44 @@
         <v>44572</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B5" s="17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="18">
-        <v>42736</v>
+        <v>44598</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>5</v>
+      <c r="D5" s="21" t="s">
+        <v>10</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="19" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" s="17">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" s="18">
-        <v>42736</v>
+        <v>44598</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
-      <c r="E6" s="20" t="s">
-        <v>10</v>
-      </c>
+      <c r="E6" s="20"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="5"/>
       <c r="B7" s="17"/>
       <c r="C7" s="18"/>
@@ -1819,7 +1814,7 @@
       <c r="E7" s="20"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="5"/>
       <c r="B8" s="17"/>
       <c r="C8" s="18"/>
@@ -1827,7 +1822,7 @@
       <c r="E8" s="20"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="5"/>
       <c r="B9" s="17"/>
       <c r="C9" s="18"/>
@@ -1835,7 +1830,7 @@
       <c r="E9" s="20"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="5"/>
       <c r="B10" s="17"/>
       <c r="C10" s="18"/>
@@ -1843,7 +1838,7 @@
       <c r="E10" s="20"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A11" s="5"/>
       <c r="B11" s="17"/>
       <c r="C11" s="18"/>
@@ -1851,7 +1846,7 @@
       <c r="E11" s="20"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A12" s="5"/>
       <c r="B12" s="17"/>
       <c r="C12" s="18"/>
@@ -1859,7 +1854,7 @@
       <c r="E12" s="20"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A13" s="5"/>
       <c r="B13" s="17"/>
       <c r="C13" s="18"/>
@@ -1867,7 +1862,7 @@
       <c r="E13" s="20"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="5"/>
       <c r="B14" s="17"/>
       <c r="C14" s="18"/>
@@ -1875,7 +1870,7 @@
       <c r="E14" s="20"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A15" s="5"/>
       <c r="B15" s="17"/>
       <c r="C15" s="18"/>
@@ -1883,7 +1878,7 @@
       <c r="E15" s="20"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A16" s="5"/>
       <c r="B16" s="17"/>
       <c r="C16" s="18"/>
@@ -1891,7 +1886,7 @@
       <c r="E16" s="20"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A17" s="5"/>
       <c r="B17" s="17"/>
       <c r="C17" s="18"/>
@@ -1899,7 +1894,7 @@
       <c r="E17" s="20"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A18" s="5"/>
       <c r="B18" s="17"/>
       <c r="C18" s="18"/>
@@ -1907,7 +1902,7 @@
       <c r="E18" s="20"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A19" s="5"/>
       <c r="B19" s="17"/>
       <c r="C19" s="18"/>
@@ -1915,7 +1910,7 @@
       <c r="E19" s="20"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A20" s="5"/>
       <c r="B20" s="17"/>
       <c r="C20" s="18"/>
@@ -1923,7 +1918,7 @@
       <c r="E20" s="20"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A21" s="5"/>
       <c r="B21" s="17"/>
       <c r="C21" s="18"/>
@@ -1931,7 +1926,7 @@
       <c r="E21" s="20"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A22" s="5"/>
       <c r="B22" s="17"/>
       <c r="C22" s="18"/>
@@ -1939,7 +1934,7 @@
       <c r="E22" s="20"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A23" s="5"/>
       <c r="B23" s="17"/>
       <c r="C23" s="18"/>
@@ -1947,7 +1942,7 @@
       <c r="E23" s="20"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A24" s="5"/>
       <c r="B24" s="17"/>
       <c r="C24" s="18"/>
@@ -1955,7 +1950,7 @@
       <c r="E24" s="20"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A25" s="5"/>
       <c r="B25" s="17"/>
       <c r="C25" s="18"/>
@@ -1963,7 +1958,7 @@
       <c r="E25" s="20"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A26" s="5"/>
       <c r="B26" s="17"/>
       <c r="C26" s="18"/>
@@ -1971,7 +1966,7 @@
       <c r="E26" s="20"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A27" s="5"/>
       <c r="B27" s="17"/>
       <c r="C27" s="18"/>
@@ -1979,7 +1974,7 @@
       <c r="E27" s="20"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A28" s="5"/>
       <c r="B28" s="17"/>
       <c r="C28" s="18"/>
@@ -1987,7 +1982,7 @@
       <c r="E28" s="20"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="11"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -1995,20 +1990,20 @@
       <c r="E29" s="3"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="6"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -2016,7 +2011,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="6"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -2024,7 +2019,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="7"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>

</xml_diff>